<commit_message>
backup and restore main images added
</commit_message>
<xml_diff>
--- a/cmake-build-debug/results/A.xlsx
+++ b/cmake-build-debug/results/A.xlsx
@@ -156,16 +156,16 @@
     </x:row>
     <x:row>
       <x:c t="str">
-        <x:v>62.7040295451601</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>69.0708872726908</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>65.8874584089254</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>01/01/2009 12:57:09 ق.ظ</x:v>
+        <x:v>64.1535622047801</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>62.7040295451601</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>63.4287958749701</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>01/01/2009 12:57:03 ق.ظ</x:v>
       </x:c>
       <x:c t="str">
         <x:v>0</x:v>
@@ -185,88 +185,10 @@
         <x:v>58.3353783819875</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>69.0708872726908</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>63.7031328273391</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>01/01/2009 12:57:07 ق.ظ</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>-1</x:v>
-      </x:c>
-    </x:row>
-    <x:row>
-      <x:c t="str">
-        <x:v>62.7040295451601</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>69.0708872726908</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>65.8874584089254</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>01/01/2009 12:57:06 ق.ظ</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>-1</x:v>
-      </x:c>
-    </x:row>
-    <x:row>
-      <x:c t="str">
-        <x:v>62.7040295451601</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>69.0708872726908</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>65.8874584089254</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>01/01/2009 12:57:04 ق.ظ</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>-1</x:v>
-      </x:c>
-    </x:row>
-    <x:row>
-      <x:c t="str">
-        <x:v>64.1535622047801</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>62.7040295451601</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>63.4287958749701</x:v>
+        <x:v>62.7040295451601</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>60.5197039635738</x:v>
       </x:c>
       <x:c t="str">
         <x:v>01/01/2009 12:57:03 ق.ظ</x:v>
@@ -286,32 +208,6 @@
     </x:row>
     <x:row>
       <x:c t="str">
-        <x:v>58.3353783819875</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>62.7040295451601</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>60.5197039635738</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>01/01/2009 12:57:03 ق.ظ</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>-1</x:v>
-      </x:c>
-    </x:row>
-    <x:row>
-      <x:c t="str">
         <x:v>64.1535622047801</x:v>
       </x:c>
       <x:c t="str">
@@ -322,6 +218,188 @@
       </x:c>
       <x:c t="str">
         <x:v>01/01/2009 12:57:02 ق.ظ</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>-1</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c t="str">
+        <x:v>62.7040295451601</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>62.7040295451601</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>62.7040295451601</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>01/01/2009 12:56:59 ق.ظ</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>-1</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c t="str">
+        <x:v>64.1535622047801</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>62.7040295451601</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>63.4287958749701</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>01/01/2009 12:56:59 ق.ظ</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>-1</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c t="str">
+        <x:v>64.1535622047801</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>62.7040295451601</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>63.4287958749701</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>01/01/2009 12:56:58 ق.ظ</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>-1</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c t="str">
+        <x:v>56.7978904096874</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>62.7040295451601</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>59.7509599774237</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>01/01/2009 12:56:58 ق.ظ</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>-1</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c t="str">
+        <x:v>64.1535622047801</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>62.7040295451601</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>63.4287958749701</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>01/01/2009 12:56:56 ق.ظ</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>-1</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c t="str">
+        <x:v>64.1535622047801</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>62.7040295451601</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>63.4287958749701</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>01/01/2009 12:56:56 ق.ظ</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>-1</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c t="str">
+        <x:v>64.1535622047801</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>64.1535622047801</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>64.1535622047801</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>01/01/2009 12:56:55 ق.ظ</x:v>
       </x:c>
       <x:c t="str">
         <x:v>0</x:v>

</xml_diff>

<commit_message>
remove same name from xlsx
</commit_message>
<xml_diff>
--- a/cmake-build-debug/results/A.xlsx
+++ b/cmake-build-debug/results/A.xlsx
@@ -182,68 +182,16 @@
     </x:row>
     <x:row>
       <x:c t="str">
-        <x:v>64.1535622047801</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>62.7040295451601</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>63.4287958749701</x:v>
+        <x:v>58.3353783819875</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>62.7040295451601</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>60.5197039635738</x:v>
       </x:c>
       <x:c t="str">
         <x:v>01/01/2009 12:57:03 ق.ظ</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>-1</x:v>
-      </x:c>
-    </x:row>
-    <x:row>
-      <x:c t="str">
-        <x:v>58.3353783819875</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>62.7040295451601</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>60.5197039635738</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>01/01/2009 12:57:03 ق.ظ</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>-1</x:v>
-      </x:c>
-    </x:row>
-    <x:row>
-      <x:c t="str">
-        <x:v>64.1535622047801</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>62.7040295451601</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>63.4287958749701</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>01/01/2009 12:56:58 ق.ظ</x:v>
       </x:c>
       <x:c t="str">
         <x:v>0</x:v>

</xml_diff>